<commit_message>
Modified the database and related files.
Changes made to the database:
1. Deleted the record where STATE_ID=0 from all Tables.
2. Removed the columns URT, HH_NO, HH_POP from HH table.

The Schema and the file containing description of tables were modified
accordingly.
Also a small Look-Up table containing description of URT_ID was added to
the Schema.
</commit_message>
<xml_diff>
--- a/docs/HAD Master Schema.xlsx
+++ b/docs/HAD Master Schema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t>STATE_ID</t>
   </si>
@@ -90,18 +90,9 @@
     <t>URT_ID</t>
   </si>
   <si>
-    <t>URT</t>
-  </si>
-  <si>
     <t>VARCHAR</t>
   </si>
   <si>
-    <t>HH_NO</t>
-  </si>
-  <si>
-    <t>HH_POP</t>
-  </si>
-  <si>
     <t>HHSIZE_1</t>
   </si>
   <si>
@@ -166,6 +157,24 @@
   </si>
   <si>
     <t>ST_TOTAL</t>
+  </si>
+  <si>
+    <t>Description of URT_ID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -189,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +229,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -311,26 +332,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -338,6 +344,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,6 +363,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,13 +394,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>577503</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>85728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
@@ -415,13 +443,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>570075</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>151275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -464,13 +492,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -511,13 +539,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>942978</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>943770</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>10320</xdr:rowOff>
@@ -558,13 +586,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>9528</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
@@ -605,13 +633,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -652,13 +680,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>409576</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>133353</xdr:rowOff>
@@ -699,13 +727,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>3</xdr:rowOff>
@@ -736,6 +764,53 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>77788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1981201" y="2763838"/>
+          <a:ext cx="619125" cy="207962"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1032,414 +1107,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N28"/>
+  <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
-      <c r="G2" s="14" t="s">
+    <row r="2" spans="2:16">
+      <c r="I2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="2:14" ht="16.5" customHeight="1">
-      <c r="G3" s="2" t="s">
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="2:16" ht="16.5" customHeight="1">
+      <c r="I3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
-      <c r="G4" s="11" t="s">
+    <row r="4" spans="2:16">
+      <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="J4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="2:16">
+      <c r="E5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="15"/>
+      <c r="N5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="2:16" ht="15" customHeight="1">
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="N7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="N12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="2:16">
+      <c r="E13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="N13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="N15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="2:14">
-      <c r="C5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="12" t="s">
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="B17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="L5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="2:14" ht="15" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="K17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="9">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="J19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="L7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="L12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="C13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="L13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="L15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="14" t="s">
+    <row r="20" spans="2:16">
+      <c r="B20" s="9">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="3:14">
-      <c r="C17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14">
-      <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="J20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="3:14">
-      <c r="C19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="J21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14">
-      <c r="C20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="J22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="E23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14">
-      <c r="C21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="J23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14">
-      <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="J24" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="E25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14">
-      <c r="C23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="J25" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="I26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="3:14">
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14">
-      <c r="C25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="3:14">
-      <c r="C26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14">
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14">
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="E6:E7"/>
+  <mergeCells count="12">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>